<commit_message>
up ok HMI PLC
</commit_message>
<xml_diff>
--- a/20231105_MrThamTraiHeoTinhVinhPhuc11/info/QuiDinhDiaChi1.xlsx
+++ b/20231105_MrThamTraiHeoTinhVinhPhuc11/info/QuiDinhDiaChi1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyCompany\8.SourceCode\3.Projects\20231101_MrThamHiTech4P\20231105_MrThamTraiHeoTinhVinhPhuc11\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F04FD48-41D2-4D33-BD53-4F5A6893EC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A08A211-FB64-4F06-9BC5-8C4D1F0C5E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="688">
   <si>
     <t>Address</t>
   </si>
@@ -1901,45 +1901,6 @@
     <t>HAW189</t>
   </si>
   <si>
-    <t>HAW190</t>
-  </si>
-  <si>
-    <t>HAW191</t>
-  </si>
-  <si>
-    <t>HAW192</t>
-  </si>
-  <si>
-    <t>HAW193</t>
-  </si>
-  <si>
-    <t>HAW194</t>
-  </si>
-  <si>
-    <t>HAW195</t>
-  </si>
-  <si>
-    <t>HAW196</t>
-  </si>
-  <si>
-    <t>HAW197</t>
-  </si>
-  <si>
-    <t>HAW198</t>
-  </si>
-  <si>
-    <t>HAW199</t>
-  </si>
-  <si>
-    <t>HAW200</t>
-  </si>
-  <si>
-    <t>HAW201</t>
-  </si>
-  <si>
-    <t>HAW202</t>
-  </si>
-  <si>
     <t>Moc1QuatCoDinh1</t>
   </si>
   <si>
@@ -1952,183 +1913,6 @@
     <t>Moc1QuatCoDinh4</t>
   </si>
   <si>
-    <t>Moc2QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc2QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc2QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc2QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc3QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc3QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc3QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc3QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc4QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc4QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc4QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc4QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc5QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc5QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc5QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc5QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc6QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc6QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc6QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc6QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc7QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc7QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc7QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc7QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc8QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc8QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc8QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc8QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc9QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc9QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc9QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc9QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>Moc10QuatCoDinh1</t>
-  </si>
-  <si>
-    <t>Moc10QuatCoDinh2</t>
-  </si>
-  <si>
-    <t>Moc10QuatCoDinh3</t>
-  </si>
-  <si>
-    <t>Moc10QuatCoDinh4</t>
-  </si>
-  <si>
-    <t>HAW203</t>
-  </si>
-  <si>
-    <t>HAW204</t>
-  </si>
-  <si>
-    <t>HAW205</t>
-  </si>
-  <si>
-    <t>HAW206</t>
-  </si>
-  <si>
-    <t>HAW207</t>
-  </si>
-  <si>
-    <t>HAW208</t>
-  </si>
-  <si>
-    <t>HAW209</t>
-  </si>
-  <si>
-    <t>HAW210</t>
-  </si>
-  <si>
-    <t>HAW211</t>
-  </si>
-  <si>
-    <t>HAW212</t>
-  </si>
-  <si>
-    <t>HAW213</t>
-  </si>
-  <si>
-    <t>HAW214</t>
-  </si>
-  <si>
-    <t>HAW215</t>
-  </si>
-  <si>
-    <t>HAW216</t>
-  </si>
-  <si>
-    <t>HAW217</t>
-  </si>
-  <si>
-    <t>HAW218</t>
-  </si>
-  <si>
-    <t>HAW219</t>
-  </si>
-  <si>
-    <t>HAW220</t>
-  </si>
-  <si>
-    <t>HAW221</t>
-  </si>
-  <si>
-    <t>HAW222</t>
-  </si>
-  <si>
-    <t>HAW223</t>
-  </si>
-  <si>
-    <t>HAW224</t>
-  </si>
-  <si>
-    <t>HAW225</t>
-  </si>
-  <si>
     <t>HAW226</t>
   </si>
   <si>
@@ -2228,18 +2012,6 @@
     <t>HDX219.0</t>
   </si>
   <si>
-    <t>HDW250</t>
-  </si>
-  <si>
-    <t>HDW251</t>
-  </si>
-  <si>
-    <t>HDW252</t>
-  </si>
-  <si>
-    <t>HDW253</t>
-  </si>
-  <si>
     <t>HDX40-51</t>
   </si>
   <si>
@@ -2328,6 +2100,30 @@
   </si>
   <si>
     <t>HAW237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>HDX300.0</t>
+  </si>
+  <si>
+    <t>Reset ca bien tinh toan chayj dung dan mat</t>
+  </si>
+  <si>
+    <t>HDW270</t>
+  </si>
+  <si>
+    <t>HDW271</t>
+  </si>
+  <si>
+    <t>HDW272</t>
+  </si>
+  <si>
+    <t>HDW273</t>
+  </si>
+  <si>
+    <t>dung trong các trigger tính tần số</t>
   </si>
 </sst>
 </file>
@@ -2537,7 +2333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2564,10 +2360,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2598,11 +2397,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2885,7 +2720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM35"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:C28"/>
     </sheetView>
   </sheetViews>
@@ -2901,21 +2736,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="34.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="M1" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="M1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
       <c r="U1" t="s">
         <v>361</v>
       </c>
@@ -3587,10 +3422,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R302"/>
+  <dimension ref="A1:R268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C174" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J195" sqref="J195:P199"/>
+    <sheetView tabSelected="1" topLeftCell="C167" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J191" sqref="J191:J194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,8 +3434,8 @@
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="28.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="30" style="35" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="53.140625" customWidth="1"/>
@@ -3608,22 +3443,22 @@
     <col min="16" max="16" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="30" t="s">
         <v>455</v>
       </c>
-      <c r="O1" s="29"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="36" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="12" t="s">
@@ -3649,10 +3484,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="37" t="s">
         <v>469</v>
       </c>
       <c r="K3" s="14" t="s">
@@ -3675,10 +3510,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="37" t="s">
         <v>470</v>
       </c>
       <c r="K4" s="14" t="s">
@@ -3701,10 +3536,10 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="37" t="s">
         <v>471</v>
       </c>
       <c r="K5" s="14" t="s">
@@ -3727,10 +3562,10 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="37" t="s">
         <v>472</v>
       </c>
       <c r="K6" s="14" t="s">
@@ -3753,10 +3588,10 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="37" t="s">
         <v>473</v>
       </c>
       <c r="K7" s="14" t="s">
@@ -3779,10 +3614,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="37" t="s">
         <v>474</v>
       </c>
       <c r="K8" s="14" t="s">
@@ -3805,10 +3640,10 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="37" t="s">
         <v>475</v>
       </c>
       <c r="K9" s="14" t="s">
@@ -3831,10 +3666,10 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="37" t="s">
         <v>476</v>
       </c>
       <c r="K10" s="14" t="s">
@@ -3857,10 +3692,10 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="37" t="s">
         <v>477</v>
       </c>
       <c r="K11" s="14" t="s">
@@ -3883,10 +3718,10 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="37" t="s">
         <v>478</v>
       </c>
       <c r="K12" s="14" t="s">
@@ -3909,10 +3744,10 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="37" t="s">
         <v>479</v>
       </c>
       <c r="K13" s="14" t="s">
@@ -3935,10 +3770,10 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="37" t="s">
         <v>491</v>
       </c>
       <c r="K14" s="14" t="s">
@@ -3956,15 +3791,15 @@
       <c r="O14" s="14" t="s">
         <v>460</v>
       </c>
-      <c r="P14" s="14">
-        <v>11</v>
+      <c r="P14" s="14" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="37" t="s">
         <v>492</v>
       </c>
       <c r="K15" s="14" t="s">
@@ -3987,10 +3822,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="37" t="s">
         <v>493</v>
       </c>
       <c r="K16" s="14" t="s">
@@ -4013,10 +3848,10 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="37" t="s">
         <v>494</v>
       </c>
       <c r="K17" s="14" t="s">
@@ -4039,10 +3874,10 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="38" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="13" t="s">
@@ -4059,10 +3894,10 @@
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="37" t="s">
         <v>480</v>
       </c>
       <c r="K19" s="14" t="s">
@@ -4085,10 +3920,10 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="37" t="s">
         <v>481</v>
       </c>
       <c r="K20" s="14" t="s">
@@ -4111,10 +3946,10 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="37" t="s">
         <v>482</v>
       </c>
       <c r="K21" s="14" t="s">
@@ -4137,10 +3972,10 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="37" t="s">
         <v>483</v>
       </c>
       <c r="K22" s="14" t="s">
@@ -4163,10 +3998,10 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="37" t="s">
         <v>484</v>
       </c>
       <c r="K23" s="14" t="s">
@@ -4189,10 +4024,10 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="37" t="s">
         <v>485</v>
       </c>
       <c r="K24" s="14" t="s">
@@ -4215,10 +4050,10 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="37" t="s">
         <v>486</v>
       </c>
       <c r="K25" s="14" t="s">
@@ -4241,10 +4076,10 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="37" t="s">
         <v>487</v>
       </c>
       <c r="K26" s="14" t="s">
@@ -4267,10 +4102,10 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="37" t="s">
         <v>488</v>
       </c>
       <c r="K27" s="14" t="s">
@@ -4293,10 +4128,10 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="J28" s="14" t="s">
+      <c r="J28" s="37" t="s">
         <v>489</v>
       </c>
       <c r="K28" s="14" t="s">
@@ -4319,10 +4154,10 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
-      <c r="J29" s="14" t="s">
+      <c r="J29" s="37" t="s">
         <v>490</v>
       </c>
       <c r="K29" s="14" t="s">
@@ -4345,10 +4180,10 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
-      <c r="J30" s="18" t="s">
+      <c r="J30" s="39" t="s">
         <v>30</v>
       </c>
       <c r="K30" s="18" t="s">
@@ -4377,7 +4212,7 @@
       <c r="A31" s="15"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="39" t="s">
         <v>154</v>
       </c>
       <c r="K31" s="18" t="s">
@@ -4404,7 +4239,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="J32" s="11" t="s">
+      <c r="J32" s="40" t="s">
         <v>31</v>
       </c>
       <c r="K32" s="11" t="s">
@@ -4430,7 +4265,7 @@
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="11" t="s">
+      <c r="J33" s="40" t="s">
         <v>32</v>
       </c>
       <c r="K33" s="11" t="s">
@@ -4456,7 +4291,7 @@
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="19" t="s">
+      <c r="J34" s="41" t="s">
         <v>33</v>
       </c>
       <c r="K34" s="19" t="s">
@@ -4482,7 +4317,7 @@
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="19" t="s">
+      <c r="J35" s="41" t="s">
         <v>153</v>
       </c>
       <c r="K35" s="19" t="s">
@@ -4508,7 +4343,7 @@
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="4" t="s">
+      <c r="J36" s="17" t="s">
         <v>35</v>
       </c>
       <c r="K36" s="4" t="s">
@@ -4525,7 +4360,7 @@
       <c r="P36" s="4"/>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="17" t="s">
         <v>38</v>
       </c>
       <c r="K37" s="4" t="s">
@@ -4542,7 +4377,7 @@
       <c r="P37" s="4"/>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="4" t="s">
+      <c r="J38" s="17" t="s">
         <v>39</v>
       </c>
       <c r="K38" s="4" t="s">
@@ -4559,7 +4394,7 @@
       <c r="P38" s="4"/>
     </row>
     <row r="39" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J39" s="4" t="s">
+      <c r="J39" s="17" t="s">
         <v>278</v>
       </c>
       <c r="K39" s="4" t="s">
@@ -4576,7 +4411,7 @@
       <c r="P39" s="4"/>
     </row>
     <row r="40" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J40" s="4" t="s">
+      <c r="J40" s="17" t="s">
         <v>40</v>
       </c>
       <c r="K40" s="4" t="s">
@@ -4593,7 +4428,7 @@
       <c r="P40" s="4"/>
     </row>
     <row r="41" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J41" s="4" t="s">
+      <c r="J41" s="17" t="s">
         <v>41</v>
       </c>
       <c r="K41" s="4" t="s">
@@ -4610,7 +4445,7 @@
       <c r="P41" s="4"/>
     </row>
     <row r="42" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J42" s="4" t="s">
+      <c r="J42" s="17" t="s">
         <v>42</v>
       </c>
       <c r="K42" s="4" t="s">
@@ -4627,7 +4462,7 @@
       <c r="P42" s="4"/>
     </row>
     <row r="43" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J43" s="4" t="s">
+      <c r="J43" s="17" t="s">
         <v>43</v>
       </c>
       <c r="K43" s="4" t="s">
@@ -4644,7 +4479,7 @@
       <c r="P43" s="4"/>
     </row>
     <row r="44" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J44" s="4" t="s">
+      <c r="J44" s="17" t="s">
         <v>44</v>
       </c>
       <c r="K44" s="4" t="s">
@@ -4661,7 +4496,7 @@
       <c r="P44" s="4"/>
     </row>
     <row r="45" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J45" s="4" t="s">
+      <c r="J45" s="17" t="s">
         <v>45</v>
       </c>
       <c r="K45" s="4" t="s">
@@ -4678,7 +4513,7 @@
       <c r="P45" s="4"/>
     </row>
     <row r="46" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J46" s="4" t="s">
+      <c r="J46" s="17" t="s">
         <v>46</v>
       </c>
       <c r="K46" s="4" t="s">
@@ -4695,7 +4530,7 @@
       <c r="P46" s="4"/>
     </row>
     <row r="47" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J47" s="4" t="s">
+      <c r="J47" s="17" t="s">
         <v>47</v>
       </c>
       <c r="K47" s="4" t="s">
@@ -4712,7 +4547,7 @@
       <c r="P47" s="4"/>
     </row>
     <row r="48" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="17" t="s">
         <v>48</v>
       </c>
       <c r="K48" s="4" t="s">
@@ -4729,7 +4564,7 @@
       <c r="P48" s="4"/>
     </row>
     <row r="49" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J49" s="4" t="s">
+      <c r="J49" s="17" t="s">
         <v>49</v>
       </c>
       <c r="K49" s="4" t="s">
@@ -4746,7 +4581,7 @@
       <c r="P49" s="4"/>
     </row>
     <row r="50" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J50" s="4" t="s">
+      <c r="J50" s="17" t="s">
         <v>50</v>
       </c>
       <c r="K50" s="4" t="s">
@@ -4763,7 +4598,7 @@
       <c r="P50" s="4"/>
     </row>
     <row r="51" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J51" s="4" t="s">
+      <c r="J51" s="17" t="s">
         <v>51</v>
       </c>
       <c r="K51" s="4" t="s">
@@ -4780,7 +4615,7 @@
       <c r="P51" s="4"/>
     </row>
     <row r="52" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J52" s="4" t="s">
+      <c r="J52" s="17" t="s">
         <v>52</v>
       </c>
       <c r="K52" s="4" t="s">
@@ -4797,7 +4632,7 @@
       <c r="P52" s="4"/>
     </row>
     <row r="53" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J53" s="4" t="s">
+      <c r="J53" s="17" t="s">
         <v>53</v>
       </c>
       <c r="K53" s="4" t="s">
@@ -4814,7 +4649,7 @@
       <c r="P53" s="4"/>
     </row>
     <row r="54" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J54" s="4" t="s">
+      <c r="J54" s="17" t="s">
         <v>54</v>
       </c>
       <c r="K54" s="4" t="s">
@@ -4831,7 +4666,7 @@
       <c r="P54" s="4"/>
     </row>
     <row r="55" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J55" s="4" t="s">
+      <c r="J55" s="17" t="s">
         <v>55</v>
       </c>
       <c r="K55" s="4" t="s">
@@ -4848,7 +4683,7 @@
       <c r="P55" s="4"/>
     </row>
     <row r="56" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J56" s="4" t="s">
+      <c r="J56" s="17" t="s">
         <v>279</v>
       </c>
       <c r="K56" s="4" t="s">
@@ -4865,7 +4700,7 @@
       <c r="P56" s="4"/>
     </row>
     <row r="57" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J57" s="4" t="s">
+      <c r="J57" s="17" t="s">
         <v>56</v>
       </c>
       <c r="K57" s="4" t="s">
@@ -4882,7 +4717,7 @@
       <c r="P57" s="4"/>
     </row>
     <row r="58" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J58" s="4" t="s">
+      <c r="J58" s="17" t="s">
         <v>57</v>
       </c>
       <c r="K58" s="4" t="s">
@@ -4899,7 +4734,7 @@
       <c r="P58" s="4"/>
     </row>
     <row r="59" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J59" s="4" t="s">
+      <c r="J59" s="17" t="s">
         <v>58</v>
       </c>
       <c r="K59" s="4" t="s">
@@ -4916,7 +4751,7 @@
       <c r="P59" s="4"/>
     </row>
     <row r="60" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J60" s="4" t="s">
+      <c r="J60" s="17" t="s">
         <v>59</v>
       </c>
       <c r="K60" s="4" t="s">
@@ -4933,7 +4768,7 @@
       <c r="P60" s="4"/>
     </row>
     <row r="61" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J61" s="4" t="s">
+      <c r="J61" s="17" t="s">
         <v>60</v>
       </c>
       <c r="K61" s="4" t="s">
@@ -4950,7 +4785,7 @@
       <c r="P61" s="4"/>
     </row>
     <row r="62" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J62" s="4" t="s">
+      <c r="J62" s="17" t="s">
         <v>61</v>
       </c>
       <c r="K62" s="4" t="s">
@@ -4967,7 +4802,7 @@
       <c r="P62" s="4"/>
     </row>
     <row r="63" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J63" s="4" t="s">
+      <c r="J63" s="17" t="s">
         <v>62</v>
       </c>
       <c r="K63" s="4" t="s">
@@ -4984,7 +4819,7 @@
       <c r="P63" s="4"/>
     </row>
     <row r="64" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J64" s="4" t="s">
+      <c r="J64" s="17" t="s">
         <v>63</v>
       </c>
       <c r="K64" s="4" t="s">
@@ -5001,7 +4836,7 @@
       <c r="P64" s="4"/>
     </row>
     <row r="65" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J65" s="4" t="s">
+      <c r="J65" s="17" t="s">
         <v>64</v>
       </c>
       <c r="K65" s="4" t="s">
@@ -5018,7 +4853,7 @@
       <c r="P65" s="4"/>
     </row>
     <row r="66" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J66" s="4" t="s">
+      <c r="J66" s="17" t="s">
         <v>65</v>
       </c>
       <c r="K66" s="4" t="s">
@@ -5035,7 +4870,7 @@
       <c r="P66" s="4"/>
     </row>
     <row r="67" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J67" s="4" t="s">
+      <c r="J67" s="17" t="s">
         <v>66</v>
       </c>
       <c r="K67" s="4" t="s">
@@ -5052,7 +4887,7 @@
       <c r="P67" s="4"/>
     </row>
     <row r="68" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J68" s="4" t="s">
+      <c r="J68" s="17" t="s">
         <v>67</v>
       </c>
       <c r="K68" s="4" t="s">
@@ -5069,7 +4904,7 @@
       <c r="P68" s="4"/>
     </row>
     <row r="69" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J69" s="4" t="s">
+      <c r="J69" s="17" t="s">
         <v>68</v>
       </c>
       <c r="K69" s="4" t="s">
@@ -5086,7 +4921,7 @@
       <c r="P69" s="4"/>
     </row>
     <row r="70" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J70" s="4" t="s">
+      <c r="J70" s="17" t="s">
         <v>69</v>
       </c>
       <c r="K70" s="4" t="s">
@@ -5103,7 +4938,7 @@
       <c r="P70" s="4"/>
     </row>
     <row r="71" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J71" s="4" t="s">
+      <c r="J71" s="17" t="s">
         <v>70</v>
       </c>
       <c r="K71" s="4" t="s">
@@ -5120,7 +4955,7 @@
       <c r="P71" s="4"/>
     </row>
     <row r="72" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J72" s="4" t="s">
+      <c r="J72" s="17" t="s">
         <v>71</v>
       </c>
       <c r="K72" s="4" t="s">
@@ -5137,7 +4972,7 @@
       <c r="P72" s="4"/>
     </row>
     <row r="73" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J73" s="4" t="s">
+      <c r="J73" s="17" t="s">
         <v>280</v>
       </c>
       <c r="K73" s="4" t="s">
@@ -5154,7 +4989,7 @@
       <c r="P73" s="4"/>
     </row>
     <row r="74" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J74" s="4" t="s">
+      <c r="J74" s="17" t="s">
         <v>72</v>
       </c>
       <c r="K74" s="4" t="s">
@@ -5171,7 +5006,7 @@
       <c r="P74" s="4"/>
     </row>
     <row r="75" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J75" s="4" t="s">
+      <c r="J75" s="17" t="s">
         <v>73</v>
       </c>
       <c r="K75" s="4" t="s">
@@ -5188,7 +5023,7 @@
       <c r="P75" s="4"/>
     </row>
     <row r="76" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J76" s="4" t="s">
+      <c r="J76" s="17" t="s">
         <v>74</v>
       </c>
       <c r="K76" s="4" t="s">
@@ -5205,7 +5040,7 @@
       <c r="P76" s="4"/>
     </row>
     <row r="77" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J77" s="4" t="s">
+      <c r="J77" s="17" t="s">
         <v>75</v>
       </c>
       <c r="K77" s="4" t="s">
@@ -5222,7 +5057,7 @@
       <c r="P77" s="4"/>
     </row>
     <row r="78" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J78" s="4" t="s">
+      <c r="J78" s="17" t="s">
         <v>76</v>
       </c>
       <c r="K78" s="4" t="s">
@@ -5239,7 +5074,7 @@
       <c r="P78" s="4"/>
     </row>
     <row r="79" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J79" s="4" t="s">
+      <c r="J79" s="17" t="s">
         <v>77</v>
       </c>
       <c r="K79" s="4" t="s">
@@ -5256,7 +5091,7 @@
       <c r="P79" s="4"/>
     </row>
     <row r="80" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J80" s="4" t="s">
+      <c r="J80" s="17" t="s">
         <v>78</v>
       </c>
       <c r="K80" s="4" t="s">
@@ -5273,7 +5108,7 @@
       <c r="P80" s="4"/>
     </row>
     <row r="81" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J81" s="4" t="s">
+      <c r="J81" s="17" t="s">
         <v>79</v>
       </c>
       <c r="K81" s="4" t="s">
@@ -5290,7 +5125,7 @@
       <c r="P81" s="4"/>
     </row>
     <row r="82" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J82" s="4" t="s">
+      <c r="J82" s="17" t="s">
         <v>80</v>
       </c>
       <c r="K82" s="4" t="s">
@@ -5307,7 +5142,7 @@
       <c r="P82" s="4"/>
     </row>
     <row r="83" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J83" s="4" t="s">
+      <c r="J83" s="17" t="s">
         <v>81</v>
       </c>
       <c r="K83" s="4" t="s">
@@ -5324,7 +5159,7 @@
       <c r="P83" s="4"/>
     </row>
     <row r="84" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J84" s="4" t="s">
+      <c r="J84" s="17" t="s">
         <v>82</v>
       </c>
       <c r="K84" s="4" t="s">
@@ -5341,7 +5176,7 @@
       <c r="P84" s="4"/>
     </row>
     <row r="85" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J85" s="4" t="s">
+      <c r="J85" s="17" t="s">
         <v>83</v>
       </c>
       <c r="K85" s="4" t="s">
@@ -5358,7 +5193,7 @@
       <c r="P85" s="4"/>
     </row>
     <row r="86" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J86" s="4" t="s">
+      <c r="J86" s="17" t="s">
         <v>84</v>
       </c>
       <c r="K86" s="4" t="s">
@@ -5375,7 +5210,7 @@
       <c r="P86" s="4"/>
     </row>
     <row r="87" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J87" s="4" t="s">
+      <c r="J87" s="17" t="s">
         <v>85</v>
       </c>
       <c r="K87" s="4" t="s">
@@ -5392,7 +5227,7 @@
       <c r="P87" s="4"/>
     </row>
     <row r="88" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J88" s="4" t="s">
+      <c r="J88" s="17" t="s">
         <v>86</v>
       </c>
       <c r="K88" s="4" t="s">
@@ -5409,7 +5244,7 @@
       <c r="P88" s="4"/>
     </row>
     <row r="89" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J89" s="4" t="s">
+      <c r="J89" s="17" t="s">
         <v>87</v>
       </c>
       <c r="K89" s="4" t="s">
@@ -5426,7 +5261,7 @@
       <c r="P89" s="4"/>
     </row>
     <row r="90" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J90" s="4" t="s">
+      <c r="J90" s="17" t="s">
         <v>281</v>
       </c>
       <c r="K90" s="4" t="s">
@@ -5443,7 +5278,7 @@
       <c r="P90" s="4"/>
     </row>
     <row r="91" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J91" s="4" t="s">
+      <c r="J91" s="17" t="s">
         <v>88</v>
       </c>
       <c r="K91" s="4" t="s">
@@ -5460,7 +5295,7 @@
       <c r="P91" s="4"/>
     </row>
     <row r="92" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J92" s="4" t="s">
+      <c r="J92" s="17" t="s">
         <v>89</v>
       </c>
       <c r="K92" s="4" t="s">
@@ -5477,7 +5312,7 @@
       <c r="P92" s="4"/>
     </row>
     <row r="93" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J93" s="4" t="s">
+      <c r="J93" s="17" t="s">
         <v>90</v>
       </c>
       <c r="K93" s="4" t="s">
@@ -5494,7 +5329,7 @@
       <c r="P93" s="4"/>
     </row>
     <row r="94" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J94" s="4" t="s">
+      <c r="J94" s="17" t="s">
         <v>91</v>
       </c>
       <c r="K94" s="4" t="s">
@@ -5511,7 +5346,7 @@
       <c r="P94" s="4"/>
     </row>
     <row r="95" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J95" s="4" t="s">
+      <c r="J95" s="17" t="s">
         <v>92</v>
       </c>
       <c r="K95" s="4" t="s">
@@ -5528,7 +5363,7 @@
       <c r="P95" s="4"/>
     </row>
     <row r="96" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J96" s="4" t="s">
+      <c r="J96" s="17" t="s">
         <v>93</v>
       </c>
       <c r="K96" s="4" t="s">
@@ -5545,7 +5380,7 @@
       <c r="P96" s="4"/>
     </row>
     <row r="97" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J97" s="4" t="s">
+      <c r="J97" s="17" t="s">
         <v>94</v>
       </c>
       <c r="K97" s="4" t="s">
@@ -5562,7 +5397,7 @@
       <c r="P97" s="4"/>
     </row>
     <row r="98" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J98" s="4" t="s">
+      <c r="J98" s="17" t="s">
         <v>95</v>
       </c>
       <c r="K98" s="4" t="s">
@@ -5579,7 +5414,7 @@
       <c r="P98" s="4"/>
     </row>
     <row r="99" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J99" s="4" t="s">
+      <c r="J99" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K99" s="4" t="s">
@@ -5596,7 +5431,7 @@
       <c r="P99" s="4"/>
     </row>
     <row r="100" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J100" s="4" t="s">
+      <c r="J100" s="17" t="s">
         <v>97</v>
       </c>
       <c r="K100" s="4" t="s">
@@ -5613,7 +5448,7 @@
       <c r="P100" s="4"/>
     </row>
     <row r="101" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J101" s="4" t="s">
+      <c r="J101" s="17" t="s">
         <v>98</v>
       </c>
       <c r="K101" s="4" t="s">
@@ -5630,7 +5465,7 @@
       <c r="P101" s="4"/>
     </row>
     <row r="102" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J102" s="4" t="s">
+      <c r="J102" s="17" t="s">
         <v>99</v>
       </c>
       <c r="K102" s="4" t="s">
@@ -5647,7 +5482,7 @@
       <c r="P102" s="4"/>
     </row>
     <row r="103" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J103" s="4" t="s">
+      <c r="J103" s="17" t="s">
         <v>100</v>
       </c>
       <c r="K103" s="4" t="s">
@@ -5664,7 +5499,7 @@
       <c r="P103" s="4"/>
     </row>
     <row r="104" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J104" s="4" t="s">
+      <c r="J104" s="17" t="s">
         <v>101</v>
       </c>
       <c r="K104" s="4" t="s">
@@ -5681,7 +5516,7 @@
       <c r="P104" s="4"/>
     </row>
     <row r="105" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J105" s="4" t="s">
+      <c r="J105" s="17" t="s">
         <v>102</v>
       </c>
       <c r="K105" s="4" t="s">
@@ -5698,7 +5533,7 @@
       <c r="P105" s="4"/>
     </row>
     <row r="106" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J106" s="4" t="s">
+      <c r="J106" s="17" t="s">
         <v>103</v>
       </c>
       <c r="K106" s="4" t="s">
@@ -5715,7 +5550,7 @@
       <c r="P106" s="4"/>
     </row>
     <row r="107" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J107" s="4" t="s">
+      <c r="J107" s="17" t="s">
         <v>282</v>
       </c>
       <c r="K107" s="4" t="s">
@@ -5732,7 +5567,7 @@
       <c r="P107" s="4"/>
     </row>
     <row r="108" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J108" s="4" t="s">
+      <c r="J108" s="17" t="s">
         <v>104</v>
       </c>
       <c r="K108" s="4" t="s">
@@ -5749,7 +5584,7 @@
       <c r="P108" s="4"/>
     </row>
     <row r="109" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J109" s="4" t="s">
+      <c r="J109" s="17" t="s">
         <v>105</v>
       </c>
       <c r="K109" s="4" t="s">
@@ -5766,7 +5601,7 @@
       <c r="P109" s="4"/>
     </row>
     <row r="110" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J110" s="4" t="s">
+      <c r="J110" s="17" t="s">
         <v>106</v>
       </c>
       <c r="K110" s="4" t="s">
@@ -5783,7 +5618,7 @@
       <c r="P110" s="4"/>
     </row>
     <row r="111" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J111" s="4" t="s">
+      <c r="J111" s="17" t="s">
         <v>107</v>
       </c>
       <c r="K111" s="4" t="s">
@@ -5800,7 +5635,7 @@
       <c r="P111" s="4"/>
     </row>
     <row r="112" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J112" s="4" t="s">
+      <c r="J112" s="17" t="s">
         <v>108</v>
       </c>
       <c r="K112" s="4" t="s">
@@ -5817,7 +5652,7 @@
       <c r="P112" s="4"/>
     </row>
     <row r="113" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J113" s="4" t="s">
+      <c r="J113" s="17" t="s">
         <v>109</v>
       </c>
       <c r="K113" s="4" t="s">
@@ -5834,7 +5669,7 @@
       <c r="P113" s="4"/>
     </row>
     <row r="114" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J114" s="4" t="s">
+      <c r="J114" s="17" t="s">
         <v>110</v>
       </c>
       <c r="K114" s="4" t="s">
@@ -5851,7 +5686,7 @@
       <c r="P114" s="4"/>
     </row>
     <row r="115" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J115" s="4" t="s">
+      <c r="J115" s="17" t="s">
         <v>111</v>
       </c>
       <c r="K115" s="4" t="s">
@@ -5868,7 +5703,7 @@
       <c r="P115" s="4"/>
     </row>
     <row r="116" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J116" s="4" t="s">
+      <c r="J116" s="17" t="s">
         <v>112</v>
       </c>
       <c r="K116" s="4" t="s">
@@ -5885,7 +5720,7 @@
       <c r="P116" s="4"/>
     </row>
     <row r="117" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J117" s="4" t="s">
+      <c r="J117" s="17" t="s">
         <v>113</v>
       </c>
       <c r="K117" s="4" t="s">
@@ -5902,7 +5737,7 @@
       <c r="P117" s="4"/>
     </row>
     <row r="118" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J118" s="4" t="s">
+      <c r="J118" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K118" s="4" t="s">
@@ -5919,7 +5754,7 @@
       <c r="P118" s="4"/>
     </row>
     <row r="119" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J119" s="4" t="s">
+      <c r="J119" s="17" t="s">
         <v>115</v>
       </c>
       <c r="K119" s="4" t="s">
@@ -5936,7 +5771,7 @@
       <c r="P119" s="4"/>
     </row>
     <row r="120" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J120" s="4" t="s">
+      <c r="J120" s="17" t="s">
         <v>116</v>
       </c>
       <c r="K120" s="4" t="s">
@@ -5953,7 +5788,7 @@
       <c r="P120" s="4"/>
     </row>
     <row r="121" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J121" s="4" t="s">
+      <c r="J121" s="17" t="s">
         <v>117</v>
       </c>
       <c r="K121" s="4" t="s">
@@ -5970,7 +5805,7 @@
       <c r="P121" s="4"/>
     </row>
     <row r="122" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J122" s="4" t="s">
+      <c r="J122" s="17" t="s">
         <v>118</v>
       </c>
       <c r="K122" s="4" t="s">
@@ -5987,7 +5822,7 @@
       <c r="P122" s="4"/>
     </row>
     <row r="123" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J123" s="4" t="s">
+      <c r="J123" s="17" t="s">
         <v>119</v>
       </c>
       <c r="K123" s="4" t="s">
@@ -6004,7 +5839,7 @@
       <c r="P123" s="4"/>
     </row>
     <row r="124" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J124" s="4" t="s">
+      <c r="J124" s="17" t="s">
         <v>283</v>
       </c>
       <c r="K124" s="4" t="s">
@@ -6021,7 +5856,7 @@
       <c r="P124" s="4"/>
     </row>
     <row r="125" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J125" s="4" t="s">
+      <c r="J125" s="17" t="s">
         <v>120</v>
       </c>
       <c r="K125" s="4" t="s">
@@ -6038,7 +5873,7 @@
       <c r="P125" s="4"/>
     </row>
     <row r="126" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J126" s="4" t="s">
+      <c r="J126" s="17" t="s">
         <v>121</v>
       </c>
       <c r="K126" s="4" t="s">
@@ -6055,7 +5890,7 @@
       <c r="P126" s="4"/>
     </row>
     <row r="127" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J127" s="4" t="s">
+      <c r="J127" s="17" t="s">
         <v>122</v>
       </c>
       <c r="K127" s="4" t="s">
@@ -6072,7 +5907,7 @@
       <c r="P127" s="4"/>
     </row>
     <row r="128" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J128" s="4" t="s">
+      <c r="J128" s="17" t="s">
         <v>123</v>
       </c>
       <c r="K128" s="4" t="s">
@@ -6089,7 +5924,7 @@
       <c r="P128" s="4"/>
     </row>
     <row r="129" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J129" s="4" t="s">
+      <c r="J129" s="17" t="s">
         <v>124</v>
       </c>
       <c r="K129" s="4" t="s">
@@ -6106,7 +5941,7 @@
       <c r="P129" s="4"/>
     </row>
     <row r="130" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J130" s="4" t="s">
+      <c r="J130" s="17" t="s">
         <v>125</v>
       </c>
       <c r="K130" s="4" t="s">
@@ -6123,7 +5958,7 @@
       <c r="P130" s="4"/>
     </row>
     <row r="131" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J131" s="4" t="s">
+      <c r="J131" s="17" t="s">
         <v>126</v>
       </c>
       <c r="K131" s="4" t="s">
@@ -6140,7 +5975,7 @@
       <c r="P131" s="4"/>
     </row>
     <row r="132" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J132" s="4" t="s">
+      <c r="J132" s="17" t="s">
         <v>127</v>
       </c>
       <c r="K132" s="4" t="s">
@@ -6157,7 +5992,7 @@
       <c r="P132" s="4"/>
     </row>
     <row r="133" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J133" s="4" t="s">
+      <c r="J133" s="17" t="s">
         <v>128</v>
       </c>
       <c r="K133" s="4" t="s">
@@ -6174,7 +6009,7 @@
       <c r="P133" s="4"/>
     </row>
     <row r="134" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J134" s="4" t="s">
+      <c r="J134" s="17" t="s">
         <v>129</v>
       </c>
       <c r="K134" s="4" t="s">
@@ -6191,7 +6026,7 @@
       <c r="P134" s="4"/>
     </row>
     <row r="135" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J135" s="4" t="s">
+      <c r="J135" s="17" t="s">
         <v>130</v>
       </c>
       <c r="K135" s="4" t="s">
@@ -6208,7 +6043,7 @@
       <c r="P135" s="4"/>
     </row>
     <row r="136" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J136" s="4" t="s">
+      <c r="J136" s="17" t="s">
         <v>131</v>
       </c>
       <c r="K136" s="4" t="s">
@@ -6225,7 +6060,7 @@
       <c r="P136" s="4"/>
     </row>
     <row r="137" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J137" s="4" t="s">
+      <c r="J137" s="17" t="s">
         <v>132</v>
       </c>
       <c r="K137" s="4" t="s">
@@ -6242,7 +6077,7 @@
       <c r="P137" s="4"/>
     </row>
     <row r="138" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J138" s="4" t="s">
+      <c r="J138" s="17" t="s">
         <v>133</v>
       </c>
       <c r="K138" s="4" t="s">
@@ -6259,7 +6094,7 @@
       <c r="P138" s="4"/>
     </row>
     <row r="139" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J139" s="4" t="s">
+      <c r="J139" s="17" t="s">
         <v>134</v>
       </c>
       <c r="K139" s="4" t="s">
@@ -6276,7 +6111,7 @@
       <c r="P139" s="4"/>
     </row>
     <row r="140" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J140" s="4" t="s">
+      <c r="J140" s="17" t="s">
         <v>135</v>
       </c>
       <c r="K140" s="4" t="s">
@@ -6293,7 +6128,7 @@
       <c r="P140" s="4"/>
     </row>
     <row r="141" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J141" s="4" t="s">
+      <c r="J141" s="17" t="s">
         <v>284</v>
       </c>
       <c r="K141" s="4" t="s">
@@ -6310,7 +6145,7 @@
       <c r="P141" s="4"/>
     </row>
     <row r="142" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J142" s="4" t="s">
+      <c r="J142" s="17" t="s">
         <v>136</v>
       </c>
       <c r="K142" s="4" t="s">
@@ -6327,7 +6162,7 @@
       <c r="P142" s="4"/>
     </row>
     <row r="143" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J143" s="4" t="s">
+      <c r="J143" s="17" t="s">
         <v>137</v>
       </c>
       <c r="K143" s="4" t="s">
@@ -6344,7 +6179,7 @@
       <c r="P143" s="4"/>
     </row>
     <row r="144" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J144" s="4" t="s">
+      <c r="J144" s="17" t="s">
         <v>138</v>
       </c>
       <c r="K144" s="4" t="s">
@@ -6361,7 +6196,7 @@
       <c r="P144" s="4"/>
     </row>
     <row r="145" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J145" s="4" t="s">
+      <c r="J145" s="17" t="s">
         <v>139</v>
       </c>
       <c r="K145" s="4" t="s">
@@ -6378,7 +6213,7 @@
       <c r="P145" s="4"/>
     </row>
     <row r="146" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J146" s="4" t="s">
+      <c r="J146" s="17" t="s">
         <v>140</v>
       </c>
       <c r="K146" s="4" t="s">
@@ -6395,7 +6230,7 @@
       <c r="P146" s="4"/>
     </row>
     <row r="147" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J147" s="4" t="s">
+      <c r="J147" s="17" t="s">
         <v>141</v>
       </c>
       <c r="K147" s="4" t="s">
@@ -6412,7 +6247,7 @@
       <c r="P147" s="4"/>
     </row>
     <row r="148" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J148" s="4" t="s">
+      <c r="J148" s="17" t="s">
         <v>142</v>
       </c>
       <c r="K148" s="4" t="s">
@@ -6429,7 +6264,7 @@
       <c r="P148" s="4"/>
     </row>
     <row r="149" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J149" s="4" t="s">
+      <c r="J149" s="17" t="s">
         <v>143</v>
       </c>
       <c r="K149" s="4" t="s">
@@ -6446,7 +6281,7 @@
       <c r="P149" s="4"/>
     </row>
     <row r="150" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J150" s="4" t="s">
+      <c r="J150" s="17" t="s">
         <v>144</v>
       </c>
       <c r="K150" s="4" t="s">
@@ -6463,7 +6298,7 @@
       <c r="P150" s="4"/>
     </row>
     <row r="151" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J151" s="4" t="s">
+      <c r="J151" s="17" t="s">
         <v>145</v>
       </c>
       <c r="K151" s="4" t="s">
@@ -6480,7 +6315,7 @@
       <c r="P151" s="4"/>
     </row>
     <row r="152" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J152" s="4" t="s">
+      <c r="J152" s="17" t="s">
         <v>146</v>
       </c>
       <c r="K152" s="4" t="s">
@@ -6497,7 +6332,7 @@
       <c r="P152" s="4"/>
     </row>
     <row r="153" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J153" s="4" t="s">
+      <c r="J153" s="17" t="s">
         <v>147</v>
       </c>
       <c r="K153" s="4" t="s">
@@ -6514,7 +6349,7 @@
       <c r="P153" s="4"/>
     </row>
     <row r="154" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J154" s="4" t="s">
+      <c r="J154" s="17" t="s">
         <v>148</v>
       </c>
       <c r="K154" s="4" t="s">
@@ -6531,7 +6366,7 @@
       <c r="P154" s="4"/>
     </row>
     <row r="155" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J155" s="4" t="s">
+      <c r="J155" s="17" t="s">
         <v>149</v>
       </c>
       <c r="K155" s="4" t="s">
@@ -6548,7 +6383,7 @@
       <c r="P155" s="4"/>
     </row>
     <row r="156" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J156" s="4" t="s">
+      <c r="J156" s="17" t="s">
         <v>276</v>
       </c>
       <c r="K156" s="4" t="s">
@@ -6565,7 +6400,7 @@
       <c r="P156" s="4"/>
     </row>
     <row r="157" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J157" s="4" t="s">
+      <c r="J157" s="17" t="s">
         <v>309</v>
       </c>
       <c r="K157" s="4" t="s">
@@ -6582,7 +6417,7 @@
       <c r="P157" s="4"/>
     </row>
     <row r="158" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J158" s="4" t="s">
+      <c r="J158" s="17" t="s">
         <v>311</v>
       </c>
       <c r="K158" s="4" t="s">
@@ -6599,7 +6434,7 @@
       <c r="P158" s="4"/>
     </row>
     <row r="159" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J159" s="4" t="s">
+      <c r="J159" s="17" t="s">
         <v>357</v>
       </c>
       <c r="K159" s="4" t="s">
@@ -6616,7 +6451,7 @@
       <c r="P159" s="4"/>
     </row>
     <row r="160" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J160" s="11" t="s">
+      <c r="J160" s="40" t="s">
         <v>359</v>
       </c>
       <c r="K160" s="11" t="s">
@@ -6640,14 +6475,14 @@
       </c>
     </row>
     <row r="161" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I161" s="30" t="s">
-        <v>707</v>
-      </c>
-      <c r="J161" s="12" t="s">
+      <c r="I161" s="31" t="s">
+        <v>635</v>
+      </c>
+      <c r="J161" s="36" t="s">
         <v>346</v>
       </c>
       <c r="K161" s="12" t="s">
-        <v>726</v>
+        <v>650</v>
       </c>
       <c r="L161" s="12"/>
       <c r="M161" s="12" t="s">
@@ -6658,12 +6493,12 @@
       <c r="P161" s="12"/>
     </row>
     <row r="162" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I162" s="30"/>
-      <c r="J162" s="12" t="s">
+      <c r="I162" s="31"/>
+      <c r="J162" s="36" t="s">
         <v>347</v>
       </c>
       <c r="K162" s="12" t="s">
-        <v>727</v>
+        <v>651</v>
       </c>
       <c r="L162" s="12"/>
       <c r="M162" s="12" t="s">
@@ -6674,12 +6509,12 @@
       <c r="P162" s="12"/>
     </row>
     <row r="163" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I163" s="30"/>
-      <c r="J163" s="12" t="s">
+      <c r="I163" s="31"/>
+      <c r="J163" s="36" t="s">
         <v>348</v>
       </c>
       <c r="K163" s="12" t="s">
-        <v>728</v>
+        <v>652</v>
       </c>
       <c r="L163" s="12"/>
       <c r="M163" s="12" t="s">
@@ -6690,12 +6525,12 @@
       <c r="P163" s="12"/>
     </row>
     <row r="164" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I164" s="30"/>
-      <c r="J164" s="12" t="s">
+      <c r="I164" s="31"/>
+      <c r="J164" s="36" t="s">
         <v>349</v>
       </c>
       <c r="K164" s="12" t="s">
-        <v>729</v>
+        <v>653</v>
       </c>
       <c r="L164" s="12"/>
       <c r="M164" s="12" t="s">
@@ -6706,12 +6541,12 @@
       <c r="P164" s="12"/>
     </row>
     <row r="165" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I165" s="30"/>
-      <c r="J165" s="12" t="s">
+      <c r="I165" s="31"/>
+      <c r="J165" s="36" t="s">
         <v>350</v>
       </c>
       <c r="K165" s="12" t="s">
-        <v>730</v>
+        <v>654</v>
       </c>
       <c r="L165" s="12"/>
       <c r="M165" s="12" t="s">
@@ -6722,12 +6557,12 @@
       <c r="P165" s="12"/>
     </row>
     <row r="166" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I166" s="30"/>
-      <c r="J166" s="12" t="s">
+      <c r="I166" s="31"/>
+      <c r="J166" s="36" t="s">
         <v>351</v>
       </c>
       <c r="K166" s="12" t="s">
-        <v>731</v>
+        <v>655</v>
       </c>
       <c r="L166" s="12"/>
       <c r="M166" s="12" t="s">
@@ -6738,12 +6573,12 @@
       <c r="P166" s="12"/>
     </row>
     <row r="167" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I167" s="30"/>
-      <c r="J167" s="12" t="s">
+      <c r="I167" s="31"/>
+      <c r="J167" s="36" t="s">
         <v>352</v>
       </c>
       <c r="K167" s="12" t="s">
-        <v>732</v>
+        <v>656</v>
       </c>
       <c r="L167" s="12"/>
       <c r="M167" s="12" t="s">
@@ -6754,12 +6589,12 @@
       <c r="P167" s="12"/>
     </row>
     <row r="168" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I168" s="30"/>
-      <c r="J168" s="12" t="s">
-        <v>696</v>
+      <c r="I168" s="31"/>
+      <c r="J168" s="36" t="s">
+        <v>624</v>
       </c>
       <c r="K168" s="12" t="s">
-        <v>733</v>
+        <v>657</v>
       </c>
       <c r="L168" s="12"/>
       <c r="M168" s="12" t="s">
@@ -6770,12 +6605,12 @@
       <c r="P168" s="12"/>
     </row>
     <row r="169" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I169" s="30"/>
-      <c r="J169" s="12" t="s">
-        <v>697</v>
+      <c r="I169" s="31"/>
+      <c r="J169" s="36" t="s">
+        <v>625</v>
       </c>
       <c r="K169" s="12" t="s">
-        <v>734</v>
+        <v>658</v>
       </c>
       <c r="L169" s="12"/>
       <c r="M169" s="12" t="s">
@@ -6786,12 +6621,12 @@
       <c r="P169" s="12"/>
     </row>
     <row r="170" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I170" s="30"/>
-      <c r="J170" s="12" t="s">
-        <v>698</v>
+      <c r="I170" s="31"/>
+      <c r="J170" s="36" t="s">
+        <v>626</v>
       </c>
       <c r="K170" s="12" t="s">
-        <v>735</v>
+        <v>659</v>
       </c>
       <c r="L170" s="12"/>
       <c r="M170" s="12" t="s">
@@ -6802,14 +6637,14 @@
       <c r="P170" s="12"/>
     </row>
     <row r="171" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I171" s="30" t="s">
-        <v>706</v>
-      </c>
-      <c r="J171" s="12" t="s">
+      <c r="I171" s="31" t="s">
+        <v>634</v>
+      </c>
+      <c r="J171" s="36" t="s">
         <v>346</v>
       </c>
       <c r="K171" s="12" t="s">
-        <v>699</v>
+        <v>627</v>
       </c>
       <c r="L171" s="12"/>
       <c r="M171" s="12" t="s">
@@ -6820,12 +6655,12 @@
       <c r="P171" s="12"/>
     </row>
     <row r="172" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I172" s="30"/>
-      <c r="J172" s="12" t="s">
+      <c r="I172" s="31"/>
+      <c r="J172" s="36" t="s">
         <v>347</v>
       </c>
       <c r="K172" s="12" t="s">
-        <v>700</v>
+        <v>628</v>
       </c>
       <c r="L172" s="12"/>
       <c r="M172" s="12" t="s">
@@ -6836,12 +6671,12 @@
       <c r="P172" s="12"/>
     </row>
     <row r="173" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I173" s="30"/>
-      <c r="J173" s="12" t="s">
+      <c r="I173" s="31"/>
+      <c r="J173" s="36" t="s">
         <v>348</v>
       </c>
       <c r="K173" s="12" t="s">
-        <v>701</v>
+        <v>629</v>
       </c>
       <c r="L173" s="12"/>
       <c r="M173" s="12" t="s">
@@ -6852,12 +6687,12 @@
       <c r="P173" s="12"/>
     </row>
     <row r="174" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I174" s="30"/>
-      <c r="J174" s="12" t="s">
+      <c r="I174" s="31"/>
+      <c r="J174" s="36" t="s">
         <v>349</v>
       </c>
       <c r="K174" s="12" t="s">
-        <v>702</v>
+        <v>630</v>
       </c>
       <c r="L174" s="12"/>
       <c r="M174" s="12" t="s">
@@ -6868,12 +6703,12 @@
       <c r="P174" s="12"/>
     </row>
     <row r="175" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I175" s="30"/>
-      <c r="J175" s="12" t="s">
+      <c r="I175" s="31"/>
+      <c r="J175" s="36" t="s">
         <v>350</v>
       </c>
       <c r="K175" s="12" t="s">
-        <v>703</v>
+        <v>631</v>
       </c>
       <c r="L175" s="12"/>
       <c r="M175" s="12" t="s">
@@ -6884,12 +6719,12 @@
       <c r="P175" s="12"/>
     </row>
     <row r="176" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I176" s="30"/>
-      <c r="J176" s="12" t="s">
+      <c r="I176" s="31"/>
+      <c r="J176" s="36" t="s">
         <v>351</v>
       </c>
       <c r="K176" s="12" t="s">
-        <v>704</v>
+        <v>632</v>
       </c>
       <c r="L176" s="12"/>
       <c r="M176" s="12" t="s">
@@ -6900,12 +6735,12 @@
       <c r="P176" s="12"/>
     </row>
     <row r="177" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I177" s="30"/>
-      <c r="J177" s="12" t="s">
+      <c r="I177" s="31"/>
+      <c r="J177" s="36" t="s">
         <v>352</v>
       </c>
       <c r="K177" s="12" t="s">
-        <v>705</v>
+        <v>633</v>
       </c>
       <c r="L177" s="12"/>
       <c r="M177" s="12" t="s">
@@ -6916,12 +6751,12 @@
       <c r="P177" s="12"/>
     </row>
     <row r="178" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I178" s="30"/>
-      <c r="J178" s="12" t="s">
-        <v>696</v>
+      <c r="I178" s="31"/>
+      <c r="J178" s="36" t="s">
+        <v>624</v>
       </c>
       <c r="K178" s="12" t="s">
-        <v>708</v>
+        <v>636</v>
       </c>
       <c r="L178" s="12"/>
       <c r="M178" s="12" t="s">
@@ -6932,12 +6767,12 @@
       <c r="P178" s="12"/>
     </row>
     <row r="179" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I179" s="30"/>
-      <c r="J179" s="12" t="s">
-        <v>697</v>
+      <c r="I179" s="31"/>
+      <c r="J179" s="36" t="s">
+        <v>625</v>
       </c>
       <c r="K179" s="12" t="s">
-        <v>709</v>
+        <v>637</v>
       </c>
       <c r="L179" s="12"/>
       <c r="M179" s="12" t="s">
@@ -6948,12 +6783,12 @@
       <c r="P179" s="12"/>
     </row>
     <row r="180" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I180" s="30"/>
-      <c r="J180" s="12" t="s">
-        <v>698</v>
+      <c r="I180" s="31"/>
+      <c r="J180" s="36" t="s">
+        <v>626</v>
       </c>
       <c r="K180" s="12" t="s">
-        <v>710</v>
+        <v>638</v>
       </c>
       <c r="L180" s="12"/>
       <c r="M180" s="12" t="s">
@@ -6964,14 +6799,14 @@
       <c r="P180" s="12"/>
     </row>
     <row r="181" spans="9:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I181" s="31" t="s">
-        <v>711</v>
-      </c>
-      <c r="J181" s="12" t="s">
+      <c r="I181" s="32" t="s">
+        <v>639</v>
+      </c>
+      <c r="J181" s="36" t="s">
         <v>346</v>
       </c>
       <c r="K181" s="12" t="s">
-        <v>712</v>
+        <v>640</v>
       </c>
       <c r="L181" s="12"/>
       <c r="M181" s="12" t="s">
@@ -6982,12 +6817,12 @@
       <c r="P181" s="12"/>
     </row>
     <row r="182" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I182" s="31"/>
-      <c r="J182" s="12" t="s">
+      <c r="I182" s="32"/>
+      <c r="J182" s="36" t="s">
         <v>347</v>
       </c>
       <c r="K182" s="12" t="s">
-        <v>713</v>
+        <v>641</v>
       </c>
       <c r="L182" s="12"/>
       <c r="M182" s="12" t="s">
@@ -6998,12 +6833,12 @@
       <c r="P182" s="12"/>
     </row>
     <row r="183" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I183" s="31"/>
-      <c r="J183" s="12" t="s">
+      <c r="I183" s="32"/>
+      <c r="J183" s="36" t="s">
         <v>348</v>
       </c>
       <c r="K183" s="12" t="s">
-        <v>714</v>
+        <v>642</v>
       </c>
       <c r="L183" s="12"/>
       <c r="M183" s="12" t="s">
@@ -7014,12 +6849,12 @@
       <c r="P183" s="12"/>
     </row>
     <row r="184" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I184" s="31"/>
-      <c r="J184" s="12" t="s">
+      <c r="I184" s="32"/>
+      <c r="J184" s="36" t="s">
         <v>349</v>
       </c>
       <c r="K184" s="12" t="s">
-        <v>715</v>
+        <v>643</v>
       </c>
       <c r="L184" s="12"/>
       <c r="M184" s="12" t="s">
@@ -7030,12 +6865,12 @@
       <c r="P184" s="12"/>
     </row>
     <row r="185" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I185" s="31"/>
-      <c r="J185" s="12" t="s">
+      <c r="I185" s="32"/>
+      <c r="J185" s="36" t="s">
         <v>350</v>
       </c>
       <c r="K185" s="12" t="s">
-        <v>716</v>
+        <v>644</v>
       </c>
       <c r="L185" s="12"/>
       <c r="M185" s="12" t="s">
@@ -7046,12 +6881,12 @@
       <c r="P185" s="12"/>
     </row>
     <row r="186" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I186" s="31"/>
-      <c r="J186" s="12" t="s">
+      <c r="I186" s="32"/>
+      <c r="J186" s="36" t="s">
         <v>351</v>
       </c>
       <c r="K186" s="12" t="s">
-        <v>717</v>
+        <v>645</v>
       </c>
       <c r="L186" s="12"/>
       <c r="M186" s="12" t="s">
@@ -7062,12 +6897,12 @@
       <c r="P186" s="12"/>
     </row>
     <row r="187" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I187" s="31"/>
-      <c r="J187" s="12" t="s">
+      <c r="I187" s="32"/>
+      <c r="J187" s="36" t="s">
         <v>352</v>
       </c>
       <c r="K187" s="12" t="s">
-        <v>718</v>
+        <v>646</v>
       </c>
       <c r="L187" s="12"/>
       <c r="M187" s="12" t="s">
@@ -7078,12 +6913,12 @@
       <c r="P187" s="12"/>
     </row>
     <row r="188" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I188" s="31"/>
-      <c r="J188" s="12" t="s">
-        <v>696</v>
+      <c r="I188" s="32"/>
+      <c r="J188" s="36" t="s">
+        <v>624</v>
       </c>
       <c r="K188" s="12" t="s">
-        <v>719</v>
+        <v>647</v>
       </c>
       <c r="L188" s="12"/>
       <c r="M188" s="12" t="s">
@@ -7094,12 +6929,12 @@
       <c r="P188" s="12"/>
     </row>
     <row r="189" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I189" s="31"/>
-      <c r="J189" s="12" t="s">
-        <v>697</v>
+      <c r="I189" s="32"/>
+      <c r="J189" s="36" t="s">
+        <v>625</v>
       </c>
       <c r="K189" s="12" t="s">
-        <v>720</v>
+        <v>648</v>
       </c>
       <c r="L189" s="12"/>
       <c r="M189" s="12" t="s">
@@ -7110,12 +6945,12 @@
       <c r="P189" s="12"/>
     </row>
     <row r="190" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I190" s="31"/>
-      <c r="J190" s="12" t="s">
-        <v>698</v>
+      <c r="I190" s="32"/>
+      <c r="J190" s="36" t="s">
+        <v>626</v>
       </c>
       <c r="K190" s="12" t="s">
-        <v>721</v>
+        <v>649</v>
       </c>
       <c r="L190" s="12"/>
       <c r="M190" s="12" t="s">
@@ -7126,10 +6961,12 @@
       <c r="P190" s="12"/>
     </row>
     <row r="191" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I191" s="31"/>
-      <c r="J191" s="12"/>
+      <c r="I191" s="32"/>
+      <c r="J191" s="45" t="s">
+        <v>687</v>
+      </c>
       <c r="K191" s="12" t="s">
-        <v>722</v>
+        <v>683</v>
       </c>
       <c r="L191" s="12"/>
       <c r="M191" s="12" t="s">
@@ -7140,10 +6977,10 @@
       <c r="P191" s="12"/>
     </row>
     <row r="192" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I192" s="31"/>
-      <c r="J192" s="12"/>
+      <c r="I192" s="32"/>
+      <c r="J192" s="46"/>
       <c r="K192" s="12" t="s">
-        <v>723</v>
+        <v>684</v>
       </c>
       <c r="L192" s="12"/>
       <c r="M192" s="12" t="s">
@@ -7154,10 +6991,10 @@
       <c r="P192" s="12"/>
     </row>
     <row r="193" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I193" s="31"/>
-      <c r="J193" s="12"/>
+      <c r="I193" s="32"/>
+      <c r="J193" s="46"/>
       <c r="K193" s="12" t="s">
-        <v>724</v>
+        <v>685</v>
       </c>
       <c r="L193" s="12"/>
       <c r="M193" s="12" t="s">
@@ -7168,10 +7005,10 @@
       <c r="P193" s="12"/>
     </row>
     <row r="194" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I194" s="31"/>
-      <c r="J194" s="12"/>
+      <c r="I194" s="32"/>
+      <c r="J194" s="47"/>
       <c r="K194" s="12" t="s">
-        <v>725</v>
+        <v>686</v>
       </c>
       <c r="L194" s="12"/>
       <c r="M194" s="12" t="s">
@@ -7181,122 +7018,119 @@
       <c r="O194" s="12"/>
       <c r="P194" s="12"/>
     </row>
-    <row r="195" spans="9:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I195" s="30" t="s">
+    <row r="195" spans="9:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="I195" s="21"/>
+      <c r="J195" s="36" t="s">
+        <v>682</v>
+      </c>
+      <c r="K195" s="12" t="s">
+        <v>681</v>
+      </c>
+      <c r="L195" s="12"/>
+      <c r="M195" s="12"/>
+      <c r="N195" s="12"/>
+      <c r="O195" s="12"/>
+      <c r="P195" s="12"/>
+    </row>
+    <row r="196" spans="9:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I196" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="J195" s="35" t="s">
+      <c r="J196" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="K195" s="35" t="s">
+      <c r="K196" s="22" t="s">
         <v>500</v>
       </c>
-      <c r="L195" s="35">
+      <c r="L196" s="22">
         <v>26</v>
       </c>
-      <c r="M195" s="35" t="s">
+      <c r="M196" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="N195" s="35"/>
-      <c r="O195" s="35"/>
-      <c r="P195" s="35"/>
-    </row>
-    <row r="196" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I196" s="30"/>
-      <c r="J196" s="35" t="s">
+      <c r="N196" s="22"/>
+      <c r="O196" s="22"/>
+      <c r="P196" s="22"/>
+    </row>
+    <row r="197" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I197" s="31"/>
+      <c r="J197" s="42" t="s">
         <v>496</v>
       </c>
-      <c r="K196" s="35" t="s">
+      <c r="K197" s="22" t="s">
         <v>501</v>
       </c>
-      <c r="L196" s="35">
+      <c r="L197" s="22">
         <v>27</v>
       </c>
-      <c r="M196" s="35" t="s">
+      <c r="M197" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="N196" s="35"/>
-      <c r="O196" s="35"/>
-      <c r="P196" s="35"/>
-    </row>
-    <row r="197" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I197" s="30"/>
-      <c r="J197" s="35" t="s">
+      <c r="N197" s="22"/>
+      <c r="O197" s="22"/>
+      <c r="P197" s="22"/>
+    </row>
+    <row r="198" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I198" s="31"/>
+      <c r="J198" s="42" t="s">
         <v>497</v>
       </c>
-      <c r="K197" s="35" t="s">
+      <c r="K198" s="22" t="s">
         <v>502</v>
       </c>
-      <c r="L197" s="35">
+      <c r="L198" s="22">
         <v>28</v>
       </c>
-      <c r="M197" s="35" t="s">
+      <c r="M198" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="N197" s="35"/>
-      <c r="O197" s="35"/>
-      <c r="P197" s="35"/>
-    </row>
-    <row r="198" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I198" s="30"/>
-      <c r="J198" s="35" t="s">
+      <c r="N198" s="22"/>
+      <c r="O198" s="22"/>
+      <c r="P198" s="22"/>
+    </row>
+    <row r="199" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I199" s="31"/>
+      <c r="J199" s="42" t="s">
         <v>498</v>
       </c>
-      <c r="K198" s="35" t="s">
+      <c r="K199" s="22" t="s">
         <v>503</v>
       </c>
-      <c r="L198" s="35">
+      <c r="L199" s="22">
         <v>131</v>
       </c>
-      <c r="M198" s="35" t="s">
+      <c r="M199" s="22" t="s">
         <v>506</v>
       </c>
-      <c r="N198" s="35"/>
-      <c r="O198" s="35"/>
-      <c r="P198" s="35"/>
-    </row>
-    <row r="199" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I199" s="30"/>
-      <c r="J199" s="35" t="s">
+      <c r="N199" s="22"/>
+      <c r="O199" s="22"/>
+      <c r="P199" s="22"/>
+    </row>
+    <row r="200" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I200" s="31"/>
+      <c r="J200" s="42" t="s">
         <v>499</v>
       </c>
-      <c r="K199" s="35" t="s">
+      <c r="K200" s="22" t="s">
         <v>504</v>
       </c>
-      <c r="L199" s="35">
+      <c r="L200" s="22">
         <v>132</v>
       </c>
-      <c r="M199" s="35"/>
-      <c r="N199" s="35"/>
-      <c r="O199" s="35"/>
-      <c r="P199" s="35"/>
-    </row>
-    <row r="200" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J200" s="4" t="s">
+      <c r="M200" s="22"/>
+      <c r="N200" s="22"/>
+      <c r="O200" s="22"/>
+      <c r="P200" s="22"/>
+    </row>
+    <row r="201" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="J201" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="K200" s="4" t="s">
+      <c r="K201" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="L200" s="4">
+      <c r="L201" s="4">
         <v>133</v>
-      </c>
-      <c r="M200" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="N200" s="4"/>
-      <c r="O200" s="4"/>
-      <c r="P200" s="4"/>
-    </row>
-    <row r="201" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J201" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="K201" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="L201" s="4">
-        <v>134</v>
       </c>
       <c r="M201" s="4" t="s">
         <v>150</v>
@@ -7306,14 +7140,14 @@
       <c r="P201" s="4"/>
     </row>
     <row r="202" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J202" s="4" t="s">
-        <v>526</v>
+      <c r="J202" s="17" t="s">
+        <v>525</v>
       </c>
       <c r="K202" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L202" s="4">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M202" s="4" t="s">
         <v>150</v>
@@ -7323,14 +7157,14 @@
       <c r="P202" s="4"/>
     </row>
     <row r="203" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J203" s="4" t="s">
-        <v>527</v>
+      <c r="J203" s="17" t="s">
+        <v>526</v>
       </c>
       <c r="K203" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L203" s="4">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M203" s="4" t="s">
         <v>150</v>
@@ -7340,14 +7174,14 @@
       <c r="P203" s="4"/>
     </row>
     <row r="204" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J204" s="4" t="s">
-        <v>528</v>
+      <c r="J204" s="17" t="s">
+        <v>527</v>
       </c>
       <c r="K204" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L204" s="4">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M204" s="4" t="s">
         <v>150</v>
@@ -7357,14 +7191,14 @@
       <c r="P204" s="4"/>
     </row>
     <row r="205" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J205" s="4" t="s">
-        <v>529</v>
+      <c r="J205" s="17" t="s">
+        <v>528</v>
       </c>
       <c r="K205" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L205" s="4">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M205" s="4" t="s">
         <v>150</v>
@@ -7374,14 +7208,14 @@
       <c r="P205" s="4"/>
     </row>
     <row r="206" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J206" s="4" t="s">
-        <v>530</v>
+      <c r="J206" s="17" t="s">
+        <v>529</v>
       </c>
       <c r="K206" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L206" s="4">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M206" s="4" t="s">
         <v>150</v>
@@ -7391,30 +7225,31 @@
       <c r="P206" s="4"/>
     </row>
     <row r="207" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J207" s="4" t="s">
-        <v>531</v>
+      <c r="J207" s="17" t="s">
+        <v>530</v>
       </c>
       <c r="K207" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L207" s="4">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M207" s="4" t="s">
         <v>150</v>
       </c>
       <c r="N207" s="4"/>
       <c r="O207" s="4"/>
+      <c r="P207" s="4"/>
     </row>
     <row r="208" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J208" s="4" t="s">
-        <v>532</v>
+      <c r="J208" s="17" t="s">
+        <v>531</v>
       </c>
       <c r="K208" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L208" s="4">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M208" s="4" t="s">
         <v>150</v>
@@ -7423,14 +7258,14 @@
       <c r="O208" s="4"/>
     </row>
     <row r="209" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J209" s="4" t="s">
-        <v>533</v>
+      <c r="J209" s="17" t="s">
+        <v>532</v>
       </c>
       <c r="K209" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L209" s="4">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M209" s="4" t="s">
         <v>150</v>
@@ -7439,14 +7274,14 @@
       <c r="O209" s="4"/>
     </row>
     <row r="210" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J210" s="4" t="s">
-        <v>534</v>
+      <c r="J210" s="17" t="s">
+        <v>533</v>
       </c>
       <c r="K210" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L210" s="4">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M210" s="4" t="s">
         <v>150</v>
@@ -7455,14 +7290,14 @@
       <c r="O210" s="4"/>
     </row>
     <row r="211" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J211" s="4" t="s">
-        <v>535</v>
+      <c r="J211" s="17" t="s">
+        <v>534</v>
       </c>
       <c r="K211" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L211" s="4">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M211" s="4" t="s">
         <v>150</v>
@@ -7471,14 +7306,14 @@
       <c r="O211" s="4"/>
     </row>
     <row r="212" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J212" s="4" t="s">
-        <v>536</v>
+      <c r="J212" s="17" t="s">
+        <v>535</v>
       </c>
       <c r="K212" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L212" s="4">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M212" s="4" t="s">
         <v>150</v>
@@ -7487,14 +7322,14 @@
       <c r="O212" s="4"/>
     </row>
     <row r="213" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J213" s="4" t="s">
-        <v>537</v>
+      <c r="J213" s="17" t="s">
+        <v>536</v>
       </c>
       <c r="K213" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L213" s="4">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M213" s="4" t="s">
         <v>150</v>
@@ -7503,14 +7338,14 @@
       <c r="O213" s="4"/>
     </row>
     <row r="214" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J214" s="4" t="s">
-        <v>538</v>
+      <c r="J214" s="17" t="s">
+        <v>537</v>
       </c>
       <c r="K214" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L214" s="4">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M214" s="4" t="s">
         <v>150</v>
@@ -7519,14 +7354,14 @@
       <c r="O214" s="4"/>
     </row>
     <row r="215" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J215" s="4" t="s">
-        <v>539</v>
+      <c r="J215" s="17" t="s">
+        <v>538</v>
       </c>
       <c r="K215" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="L215" s="4">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M215" s="4" t="s">
         <v>150</v>
@@ -7535,14 +7370,14 @@
       <c r="O215" s="4"/>
     </row>
     <row r="216" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J216" s="4" t="s">
-        <v>540</v>
+      <c r="J216" s="17" t="s">
+        <v>539</v>
       </c>
       <c r="K216" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="L216" s="4">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M216" s="4" t="s">
         <v>150</v>
@@ -7551,14 +7386,14 @@
       <c r="O216" s="4"/>
     </row>
     <row r="217" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J217" s="4" t="s">
-        <v>507</v>
+      <c r="J217" s="17" t="s">
+        <v>540</v>
       </c>
       <c r="K217" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L217" s="4">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M217" s="4" t="s">
         <v>150</v>
@@ -7567,14 +7402,14 @@
       <c r="O217" s="4"/>
     </row>
     <row r="218" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J218" s="4" t="s">
-        <v>541</v>
+      <c r="J218" s="17" t="s">
+        <v>507</v>
       </c>
       <c r="K218" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L218" s="4">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M218" s="4" t="s">
         <v>150</v>
@@ -7583,14 +7418,14 @@
       <c r="O218" s="4"/>
     </row>
     <row r="219" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J219" s="4" t="s">
-        <v>542</v>
+      <c r="J219" s="17" t="s">
+        <v>541</v>
       </c>
       <c r="K219" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L219" s="4">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M219" s="4" t="s">
         <v>150</v>
@@ -7599,14 +7434,14 @@
       <c r="O219" s="4"/>
     </row>
     <row r="220" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J220" s="4" t="s">
-        <v>543</v>
+      <c r="J220" s="17" t="s">
+        <v>542</v>
       </c>
       <c r="K220" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L220" s="4">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M220" s="4" t="s">
         <v>150</v>
@@ -7615,14 +7450,14 @@
       <c r="O220" s="4"/>
     </row>
     <row r="221" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J221" s="4" t="s">
-        <v>544</v>
+      <c r="J221" s="17" t="s">
+        <v>543</v>
       </c>
       <c r="K221" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L221" s="4">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M221" s="4" t="s">
         <v>150</v>
@@ -7631,14 +7466,14 @@
       <c r="O221" s="4"/>
     </row>
     <row r="222" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J222" s="4" t="s">
-        <v>545</v>
+      <c r="J222" s="17" t="s">
+        <v>544</v>
       </c>
       <c r="K222" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L222" s="4">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M222" s="4" t="s">
         <v>150</v>
@@ -7647,14 +7482,14 @@
       <c r="O222" s="4"/>
     </row>
     <row r="223" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J223" s="4" t="s">
-        <v>546</v>
+      <c r="J223" s="17" t="s">
+        <v>545</v>
       </c>
       <c r="K223" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L223" s="4">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M223" s="4" t="s">
         <v>150</v>
@@ -7663,14 +7498,14 @@
       <c r="O223" s="4"/>
     </row>
     <row r="224" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J224" s="4" t="s">
-        <v>547</v>
+      <c r="J224" s="17" t="s">
+        <v>546</v>
       </c>
       <c r="K224" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L224" s="4">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M224" s="4" t="s">
         <v>150</v>
@@ -7679,14 +7514,14 @@
       <c r="O224" s="4"/>
     </row>
     <row r="225" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J225" s="4" t="s">
-        <v>548</v>
+      <c r="J225" s="17" t="s">
+        <v>547</v>
       </c>
       <c r="K225" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L225" s="4">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M225" s="4" t="s">
         <v>150</v>
@@ -7695,14 +7530,14 @@
       <c r="O225" s="4"/>
     </row>
     <row r="226" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J226" s="4" t="s">
-        <v>549</v>
+      <c r="J226" s="17" t="s">
+        <v>548</v>
       </c>
       <c r="K226" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L226" s="4">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M226" s="4" t="s">
         <v>150</v>
@@ -7711,14 +7546,14 @@
       <c r="O226" s="4"/>
     </row>
     <row r="227" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J227" s="4" t="s">
-        <v>550</v>
+      <c r="J227" s="17" t="s">
+        <v>549</v>
       </c>
       <c r="K227" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L227" s="4">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M227" s="4" t="s">
         <v>150</v>
@@ -7727,14 +7562,14 @@
       <c r="O227" s="4"/>
     </row>
     <row r="228" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J228" s="4" t="s">
-        <v>551</v>
+      <c r="J228" s="17" t="s">
+        <v>550</v>
       </c>
       <c r="K228" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L228" s="4">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M228" s="4" t="s">
         <v>150</v>
@@ -7743,14 +7578,14 @@
       <c r="O228" s="4"/>
     </row>
     <row r="229" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J229" s="4" t="s">
-        <v>552</v>
+      <c r="J229" s="17" t="s">
+        <v>551</v>
       </c>
       <c r="K229" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L229" s="4">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M229" s="4" t="s">
         <v>150</v>
@@ -7759,14 +7594,14 @@
       <c r="O229" s="4"/>
     </row>
     <row r="230" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J230" s="4" t="s">
-        <v>553</v>
+      <c r="J230" s="17" t="s">
+        <v>552</v>
       </c>
       <c r="K230" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L230" s="4">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M230" s="4" t="s">
         <v>150</v>
@@ -7775,14 +7610,14 @@
       <c r="O230" s="4"/>
     </row>
     <row r="231" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J231" s="4" t="s">
-        <v>554</v>
+      <c r="J231" s="17" t="s">
+        <v>553</v>
       </c>
       <c r="K231" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L231" s="4">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M231" s="4" t="s">
         <v>150</v>
@@ -7791,14 +7626,14 @@
       <c r="O231" s="4"/>
     </row>
     <row r="232" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J232" s="4" t="s">
-        <v>555</v>
+      <c r="J232" s="17" t="s">
+        <v>554</v>
       </c>
       <c r="K232" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L232" s="4">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M232" s="4" t="s">
         <v>150</v>
@@ -7807,14 +7642,14 @@
       <c r="O232" s="4"/>
     </row>
     <row r="233" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J233" s="4" t="s">
-        <v>556</v>
+      <c r="J233" s="17" t="s">
+        <v>555</v>
       </c>
       <c r="K233" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L233" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M233" s="4" t="s">
         <v>150</v>
@@ -7823,14 +7658,14 @@
       <c r="O233" s="4"/>
     </row>
     <row r="234" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J234" s="4" t="s">
-        <v>509</v>
+      <c r="J234" s="17" t="s">
+        <v>556</v>
       </c>
       <c r="K234" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L234" s="4">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M234" s="4" t="s">
         <v>150</v>
@@ -7839,14 +7674,14 @@
       <c r="O234" s="4"/>
     </row>
     <row r="235" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J235" s="4" t="s">
-        <v>510</v>
+      <c r="J235" s="17" t="s">
+        <v>509</v>
       </c>
       <c r="K235" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L235" s="4">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M235" s="4" t="s">
         <v>150</v>
@@ -7855,14 +7690,14 @@
       <c r="O235" s="4"/>
     </row>
     <row r="236" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J236" s="4" t="s">
-        <v>511</v>
+      <c r="J236" s="17" t="s">
+        <v>510</v>
       </c>
       <c r="K236" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L236" s="4">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M236" s="4" t="s">
         <v>150</v>
@@ -7871,14 +7706,14 @@
       <c r="O236" s="4"/>
     </row>
     <row r="237" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J237" s="4" t="s">
-        <v>512</v>
+      <c r="J237" s="17" t="s">
+        <v>511</v>
       </c>
       <c r="K237" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L237" s="4">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M237" s="4" t="s">
         <v>150</v>
@@ -7887,14 +7722,14 @@
       <c r="O237" s="4"/>
     </row>
     <row r="238" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J238" s="4" t="s">
-        <v>513</v>
+      <c r="J238" s="17" t="s">
+        <v>512</v>
       </c>
       <c r="K238" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L238" s="4">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M238" s="4" t="s">
         <v>150</v>
@@ -7903,14 +7738,14 @@
       <c r="O238" s="4"/>
     </row>
     <row r="239" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J239" s="4" t="s">
-        <v>514</v>
+      <c r="J239" s="17" t="s">
+        <v>513</v>
       </c>
       <c r="K239" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L239" s="4">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M239" s="4" t="s">
         <v>150</v>
@@ -7919,14 +7754,14 @@
       <c r="O239" s="4"/>
     </row>
     <row r="240" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J240" s="4" t="s">
-        <v>695</v>
+      <c r="J240" s="17" t="s">
+        <v>514</v>
       </c>
       <c r="K240" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L240" s="4">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M240" s="4" t="s">
         <v>150</v>
@@ -7934,15 +7769,15 @@
       <c r="N240" s="4"/>
       <c r="O240" s="4"/>
     </row>
-    <row r="241" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J241" s="4" t="s">
-        <v>515</v>
+    <row r="241" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J241" s="17" t="s">
+        <v>623</v>
       </c>
       <c r="K241" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L241" s="4">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M241" s="4" t="s">
         <v>150</v>
@@ -7950,15 +7785,15 @@
       <c r="N241" s="4"/>
       <c r="O241" s="4"/>
     </row>
-    <row r="242" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J242" s="4" t="s">
-        <v>516</v>
+    <row r="242" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J242" s="17" t="s">
+        <v>515</v>
       </c>
       <c r="K242" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L242" s="4">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M242" s="4" t="s">
         <v>150</v>
@@ -7966,15 +7801,15 @@
       <c r="N242" s="4"/>
       <c r="O242" s="4"/>
     </row>
-    <row r="243" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J243" s="4" t="s">
-        <v>517</v>
+    <row r="243" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J243" s="17" t="s">
+        <v>516</v>
       </c>
       <c r="K243" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L243" s="4">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M243" s="4" t="s">
         <v>150</v>
@@ -7982,15 +7817,15 @@
       <c r="N243" s="4"/>
       <c r="O243" s="4"/>
     </row>
-    <row r="244" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J244" s="4" t="s">
-        <v>518</v>
+    <row r="244" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J244" s="17" t="s">
+        <v>517</v>
       </c>
       <c r="K244" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L244" s="4">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M244" s="4" t="s">
         <v>150</v>
@@ -7998,15 +7833,15 @@
       <c r="N244" s="4"/>
       <c r="O244" s="4"/>
     </row>
-    <row r="245" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J245" s="4" t="s">
-        <v>519</v>
+    <row r="245" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J245" s="17" t="s">
+        <v>518</v>
       </c>
       <c r="K245" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="L245" s="4">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M245" s="4" t="s">
         <v>150</v>
@@ -8014,15 +7849,15 @@
       <c r="N245" s="4"/>
       <c r="O245" s="4"/>
     </row>
-    <row r="246" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J246" s="4" t="s">
-        <v>520</v>
+    <row r="246" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J246" s="17" t="s">
+        <v>519</v>
       </c>
       <c r="K246" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="L246" s="4">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M246" s="4" t="s">
         <v>150</v>
@@ -8030,15 +7865,15 @@
       <c r="N246" s="4"/>
       <c r="O246" s="4"/>
     </row>
-    <row r="247" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J247" s="4" t="s">
-        <v>521</v>
+    <row r="247" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J247" s="17" t="s">
+        <v>520</v>
       </c>
       <c r="K247" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="L247" s="4">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M247" s="4" t="s">
         <v>150</v>
@@ -8046,15 +7881,15 @@
       <c r="N247" s="4"/>
       <c r="O247" s="4"/>
     </row>
-    <row r="248" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J248" s="4" t="s">
-        <v>522</v>
+    <row r="248" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J248" s="17" t="s">
+        <v>521</v>
       </c>
       <c r="K248" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="L248" s="4">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M248" s="4" t="s">
         <v>150</v>
@@ -8062,15 +7897,15 @@
       <c r="N248" s="4"/>
       <c r="O248" s="4"/>
     </row>
-    <row r="249" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J249" s="4" t="s">
-        <v>523</v>
+    <row r="249" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J249" s="17" t="s">
+        <v>522</v>
       </c>
       <c r="K249" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="L249" s="4">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M249" s="4" t="s">
         <v>150</v>
@@ -8078,15 +7913,15 @@
       <c r="N249" s="4"/>
       <c r="O249" s="4"/>
     </row>
-    <row r="250" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J250" s="4" t="s">
-        <v>524</v>
+    <row r="250" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J250" s="17" t="s">
+        <v>523</v>
       </c>
       <c r="K250" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="L250" s="4">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M250" s="4" t="s">
         <v>150</v>
@@ -8094,719 +7929,268 @@
       <c r="N250" s="4"/>
       <c r="O250" s="4"/>
     </row>
-    <row r="251" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J251" s="20" t="s">
-        <v>626</v>
-      </c>
-      <c r="K251" s="12" t="s">
+    <row r="251" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J251" s="17" t="s">
+        <v>524</v>
+      </c>
+      <c r="K251" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="L251" s="4">
+        <v>183</v>
+      </c>
+      <c r="M251" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N251" s="4"/>
+      <c r="O251" s="4"/>
+    </row>
+    <row r="252" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J252" s="43" t="s">
+        <v>613</v>
+      </c>
+      <c r="K252" s="12" t="s">
         <v>609</v>
       </c>
-      <c r="L251" s="4">
+      <c r="L252" s="4">
         <v>184</v>
       </c>
-      <c r="M251" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="252" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J252" s="20" t="s">
-        <v>627</v>
-      </c>
-      <c r="K252" s="12" t="s">
+      <c r="M252" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="253" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J253" s="43" t="s">
+        <v>614</v>
+      </c>
+      <c r="K253" s="12" t="s">
         <v>610</v>
       </c>
-      <c r="L252" s="4">
+      <c r="L253" s="4">
         <v>185</v>
       </c>
-      <c r="M252" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="253" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J253" s="20" t="s">
-        <v>628</v>
-      </c>
-      <c r="K253" s="12" t="s">
+      <c r="M253" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="254" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J254" s="43" t="s">
+        <v>615</v>
+      </c>
+      <c r="K254" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="L253" s="4">
+      <c r="L254" s="4">
         <v>186</v>
       </c>
-      <c r="M253" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="254" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J254" s="20" t="s">
-        <v>629</v>
-      </c>
-      <c r="K254" s="12" t="s">
+      <c r="M254" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="255" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="J255" s="43" t="s">
+        <v>616</v>
+      </c>
+      <c r="K255" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="L254" s="4">
+      <c r="L255" s="4">
         <v>187</v>
       </c>
-      <c r="M254" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="255" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J255" s="34" t="s">
-        <v>630</v>
-      </c>
-      <c r="K255" s="35" t="s">
-        <v>613</v>
-      </c>
-      <c r="L255" s="35">
-        <v>188</v>
-      </c>
-      <c r="M255" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="256" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J256" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="K256" s="35" t="s">
-        <v>614</v>
-      </c>
-      <c r="L256" s="35">
-        <v>189</v>
-      </c>
-      <c r="M256" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="257" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J257" s="34" t="s">
-        <v>632</v>
-      </c>
-      <c r="K257" s="35" t="s">
-        <v>615</v>
-      </c>
-      <c r="L257" s="35">
-        <v>190</v>
-      </c>
-      <c r="M257" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="258" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J258" s="36" t="s">
-        <v>633</v>
-      </c>
-      <c r="K258" s="35" t="s">
-        <v>616</v>
-      </c>
-      <c r="L258" s="35">
-        <v>191</v>
-      </c>
-      <c r="M258" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="259" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J259" s="34" t="s">
-        <v>634</v>
-      </c>
-      <c r="K259" s="35" t="s">
+      <c r="M255" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="256" spans="9:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I256" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="J256" s="44" t="s">
+        <v>619</v>
+      </c>
+      <c r="K256" s="12" t="s">
         <v>617</v>
       </c>
-      <c r="L259" s="35">
-        <v>192</v>
-      </c>
-      <c r="M259" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="260" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J260" s="36" t="s">
-        <v>635</v>
-      </c>
-      <c r="K260" s="35" t="s">
+      <c r="L256" s="4">
+        <v>224</v>
+      </c>
+      <c r="M256" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="257" spans="9:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="I257" s="20" t="s">
+        <v>622</v>
+      </c>
+      <c r="J257" s="44" t="s">
+        <v>620</v>
+      </c>
+      <c r="K257" s="33" t="s">
         <v>618</v>
       </c>
-      <c r="L260" s="35">
-        <v>193</v>
-      </c>
-      <c r="M260" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="261" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J261" s="34" t="s">
-        <v>636</v>
-      </c>
-      <c r="K261" s="35" t="s">
-        <v>619</v>
-      </c>
-      <c r="L261" s="35">
-        <v>194</v>
-      </c>
-      <c r="M261" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="262" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J262" s="36" t="s">
-        <v>637</v>
-      </c>
-      <c r="K262" s="35" t="s">
-        <v>620</v>
-      </c>
-      <c r="L262" s="35">
-        <v>195</v>
-      </c>
-      <c r="M262" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="263" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J263" s="34" t="s">
-        <v>638</v>
-      </c>
-      <c r="K263" s="35" t="s">
-        <v>621</v>
-      </c>
-      <c r="L263" s="35">
-        <v>196</v>
-      </c>
-      <c r="M263" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="264" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J264" s="36" t="s">
-        <v>639</v>
-      </c>
-      <c r="K264" s="35" t="s">
-        <v>622</v>
-      </c>
-      <c r="L264" s="35">
-        <v>197</v>
-      </c>
-      <c r="M264" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="265" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J265" s="34" t="s">
-        <v>640</v>
-      </c>
-      <c r="K265" s="35" t="s">
-        <v>623</v>
-      </c>
-      <c r="L265" s="35">
-        <v>198</v>
-      </c>
-      <c r="M265" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="266" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J266" s="36" t="s">
-        <v>641</v>
-      </c>
-      <c r="K266" s="35" t="s">
-        <v>624</v>
-      </c>
-      <c r="L266" s="35">
-        <v>199</v>
-      </c>
-      <c r="M266" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="267" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J267" s="34" t="s">
-        <v>642</v>
-      </c>
-      <c r="K267" s="35" t="s">
-        <v>625</v>
-      </c>
-      <c r="L267" s="35">
-        <v>200</v>
-      </c>
-      <c r="M267" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="268" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J268" s="36" t="s">
-        <v>643</v>
-      </c>
-      <c r="K268" s="35" t="s">
+      <c r="L257" s="34">
+        <v>225</v>
+      </c>
+      <c r="M257" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="258" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J258" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="K258" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="L258" s="4">
+        <v>226</v>
+      </c>
+      <c r="M258" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="259" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J259" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="K259" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="L259" s="4">
+        <v>227</v>
+      </c>
+      <c r="M259" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="260" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J260" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="K260" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="L260" s="4">
+        <v>228</v>
+      </c>
+      <c r="M260" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="261" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J261" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="K261" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="L261" s="4">
+        <v>229</v>
+      </c>
+      <c r="M261" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="262" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J262" s="17" t="s">
+        <v>664</v>
+      </c>
+      <c r="K262" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="L262" s="4">
+        <v>230</v>
+      </c>
+      <c r="M262" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="263" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J263" s="17" t="s">
+        <v>665</v>
+      </c>
+      <c r="K263" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="L263" s="4">
+        <v>231</v>
+      </c>
+      <c r="M263" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="264" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J264" s="17" t="s">
         <v>666</v>
       </c>
-      <c r="L268" s="35">
-        <v>201</v>
-      </c>
-      <c r="M268" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="269" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J269" s="34" t="s">
-        <v>644</v>
-      </c>
-      <c r="K269" s="35" t="s">
+      <c r="K264" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="L264" s="4">
+        <v>232</v>
+      </c>
+      <c r="M264" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="265" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J265" s="17" t="s">
         <v>667</v>
       </c>
-      <c r="L269" s="35">
-        <v>202</v>
-      </c>
-      <c r="M269" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="270" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J270" s="36" t="s">
-        <v>645</v>
-      </c>
-      <c r="K270" s="35" t="s">
+      <c r="K265" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="L265" s="4">
+        <v>233</v>
+      </c>
+      <c r="M265" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="266" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J266" s="17" t="s">
         <v>668</v>
       </c>
-      <c r="L270" s="35">
-        <v>203</v>
-      </c>
-      <c r="M270" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="271" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J271" s="34" t="s">
-        <v>646</v>
-      </c>
-      <c r="K271" s="35" t="s">
+      <c r="K266" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="L266" s="4">
+        <v>234</v>
+      </c>
+      <c r="M266" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="267" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J267" s="17" t="s">
         <v>669</v>
       </c>
-      <c r="L271" s="35">
-        <v>204</v>
-      </c>
-      <c r="M271" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="272" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J272" s="36" t="s">
-        <v>647</v>
-      </c>
-      <c r="K272" s="35" t="s">
-        <v>670</v>
-      </c>
-      <c r="L272" s="35">
-        <v>205</v>
-      </c>
-      <c r="M272" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="273" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J273" s="34" t="s">
-        <v>648</v>
-      </c>
-      <c r="K273" s="35" t="s">
-        <v>671</v>
-      </c>
-      <c r="L273" s="35">
-        <v>206</v>
-      </c>
-      <c r="M273" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="274" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J274" s="36" t="s">
-        <v>649</v>
-      </c>
-      <c r="K274" s="35" t="s">
-        <v>672</v>
-      </c>
-      <c r="L274" s="35">
-        <v>207</v>
-      </c>
-      <c r="M274" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="275" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J275" s="34" t="s">
-        <v>650</v>
-      </c>
-      <c r="K275" s="35" t="s">
-        <v>673</v>
-      </c>
-      <c r="L275" s="35">
-        <v>208</v>
-      </c>
-      <c r="M275" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="276" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J276" s="36" t="s">
-        <v>651</v>
-      </c>
-      <c r="K276" s="35" t="s">
-        <v>674</v>
-      </c>
-      <c r="L276" s="35">
-        <v>209</v>
-      </c>
-      <c r="M276" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="277" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J277" s="34" t="s">
-        <v>652</v>
-      </c>
-      <c r="K277" s="35" t="s">
-        <v>675</v>
-      </c>
-      <c r="L277" s="35">
-        <v>210</v>
-      </c>
-      <c r="M277" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="278" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J278" s="36" t="s">
-        <v>653</v>
-      </c>
-      <c r="K278" s="35" t="s">
-        <v>676</v>
-      </c>
-      <c r="L278" s="35">
-        <v>211</v>
-      </c>
-      <c r="M278" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="279" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J279" s="34" t="s">
-        <v>654</v>
-      </c>
-      <c r="K279" s="35" t="s">
-        <v>677</v>
-      </c>
-      <c r="L279" s="35">
-        <v>212</v>
-      </c>
-      <c r="M279" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="280" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J280" s="36" t="s">
-        <v>655</v>
-      </c>
-      <c r="K280" s="35" t="s">
-        <v>678</v>
-      </c>
-      <c r="L280" s="35">
-        <v>213</v>
-      </c>
-      <c r="M280" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="281" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J281" s="34" t="s">
-        <v>656</v>
-      </c>
-      <c r="K281" s="35" t="s">
+      <c r="K267" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="L281" s="35">
-        <v>214</v>
-      </c>
-      <c r="M281" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="282" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J282" s="36" t="s">
-        <v>657</v>
-      </c>
-      <c r="K282" s="35" t="s">
-        <v>680</v>
-      </c>
-      <c r="L282" s="35">
-        <v>215</v>
-      </c>
-      <c r="M282" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="283" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J283" s="34" t="s">
-        <v>658</v>
-      </c>
-      <c r="K283" s="35" t="s">
-        <v>681</v>
-      </c>
-      <c r="L283" s="35">
-        <v>216</v>
-      </c>
-      <c r="M283" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="284" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J284" s="36" t="s">
-        <v>659</v>
-      </c>
-      <c r="K284" s="35" t="s">
-        <v>682</v>
-      </c>
-      <c r="L284" s="35">
-        <v>217</v>
-      </c>
-      <c r="M284" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="285" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J285" s="34" t="s">
-        <v>660</v>
-      </c>
-      <c r="K285" s="35" t="s">
-        <v>683</v>
-      </c>
-      <c r="L285" s="35">
-        <v>218</v>
-      </c>
-      <c r="M285" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="286" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J286" s="36" t="s">
-        <v>661</v>
-      </c>
-      <c r="K286" s="35" t="s">
-        <v>684</v>
-      </c>
-      <c r="L286" s="35">
-        <v>219</v>
-      </c>
-      <c r="M286" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="287" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J287" s="34" t="s">
-        <v>662</v>
-      </c>
-      <c r="K287" s="35" t="s">
-        <v>685</v>
-      </c>
-      <c r="L287" s="35">
-        <v>220</v>
-      </c>
-      <c r="M287" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="288" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J288" s="36" t="s">
-        <v>663</v>
-      </c>
-      <c r="K288" s="35" t="s">
-        <v>686</v>
-      </c>
-      <c r="L288" s="35">
-        <v>221</v>
-      </c>
-      <c r="M288" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="289" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J289" s="34" t="s">
-        <v>664</v>
-      </c>
-      <c r="K289" s="35" t="s">
-        <v>687</v>
-      </c>
-      <c r="L289" s="35">
-        <v>222</v>
-      </c>
-      <c r="M289" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="290" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J290" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="K290" s="35" t="s">
-        <v>688</v>
-      </c>
-      <c r="L290" s="35">
-        <v>223</v>
-      </c>
-      <c r="M290" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="291" spans="9:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="I291" s="21" t="s">
-        <v>693</v>
-      </c>
-      <c r="J291" s="7" t="s">
-        <v>691</v>
-      </c>
-      <c r="K291" s="12" t="s">
-        <v>689</v>
-      </c>
-      <c r="L291" s="4">
-        <v>224</v>
-      </c>
-      <c r="M291" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="292" spans="9:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="I292" s="21" t="s">
-        <v>694</v>
-      </c>
-      <c r="J292" s="7" t="s">
-        <v>692</v>
-      </c>
-      <c r="K292" s="12" t="s">
-        <v>690</v>
-      </c>
-      <c r="L292" s="4">
-        <v>225</v>
-      </c>
-      <c r="M292" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="293" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J293" s="32" t="s">
-        <v>736</v>
-      </c>
-      <c r="K293" s="12" t="s">
-        <v>746</v>
-      </c>
-      <c r="L293" s="4">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="294" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J294" s="33" t="s">
-        <v>737</v>
-      </c>
-      <c r="K294" s="12" t="s">
-        <v>747</v>
-      </c>
-      <c r="L294" s="4">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="295" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J295" s="32" t="s">
-        <v>738</v>
-      </c>
-      <c r="K295" s="12" t="s">
-        <v>748</v>
-      </c>
-      <c r="L295" s="4">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="296" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J296" s="33" t="s">
-        <v>739</v>
-      </c>
-      <c r="K296" s="12" t="s">
-        <v>749</v>
-      </c>
-      <c r="L296" s="4">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="297" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J297" s="32" t="s">
-        <v>740</v>
-      </c>
-      <c r="K297" s="12" t="s">
-        <v>750</v>
-      </c>
-      <c r="L297" s="4">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="298" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J298" s="33" t="s">
-        <v>741</v>
-      </c>
-      <c r="K298" s="12" t="s">
-        <v>751</v>
-      </c>
-      <c r="L298" s="4">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="299" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J299" s="32" t="s">
-        <v>742</v>
-      </c>
-      <c r="K299" s="12" t="s">
-        <v>752</v>
-      </c>
-      <c r="L299" s="4">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="300" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J300" s="33" t="s">
-        <v>743</v>
-      </c>
-      <c r="K300" s="12" t="s">
-        <v>753</v>
-      </c>
-      <c r="L300" s="4">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="301" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J301" s="32" t="s">
-        <v>744</v>
-      </c>
-      <c r="K301" s="12" t="s">
-        <v>754</v>
-      </c>
-      <c r="L301" s="4">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="302" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J302" s="33" t="s">
-        <v>745</v>
-      </c>
-      <c r="K302" s="12" t="s">
-        <v>755</v>
-      </c>
-      <c r="L302" s="4">
+      <c r="L267" s="4">
         <v>235</v>
       </c>
+      <c r="M267" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="268" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J268" s="17"/>
+      <c r="K268" s="4"/>
+      <c r="L268" s="4"/>
+      <c r="M268" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A3:A17"/>
     <mergeCell ref="A18:A30"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="I195:I199"/>
+    <mergeCell ref="I196:I200"/>
     <mergeCell ref="I171:I180"/>
     <mergeCell ref="I161:I170"/>
     <mergeCell ref="I181:I194"/>
+    <mergeCell ref="J191:J194"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>